<commit_message>
update on objective and earliest start feature
</commit_message>
<xml_diff>
--- a/study_plan.xlsx
+++ b/study_plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cevat\Desktop\assignment\Study-Plan-Optimizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC1B79C-7C76-4968-B534-462A845DA20C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087991D0-44F7-43E3-9911-6B6F6B8ADC77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="3672" windowWidth="23256" windowHeight="12456" xr2:uid="{4083871D-627C-433C-8B17-E6F26D87DB11}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4083871D-627C-433C-8B17-E6F26D87DB11}"/>
   </bookViews>
   <sheets>
     <sheet name="Activities" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Activity</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Semester Start Date</t>
+  </si>
+  <si>
+    <t>Earliest Start Week</t>
   </si>
 </sst>
 </file>
@@ -486,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0C5FA0-D3C5-4850-8201-23CDA5D9B976}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +500,7 @@
     <col min="1" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,8 +513,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -524,8 +530,11 @@
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -538,8 +547,11 @@
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -552,8 +564,11 @@
       <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -566,8 +581,11 @@
       <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -580,8 +598,11 @@
       <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -593,6 +614,9 @@
       </c>
       <c r="D7" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -605,12 +629,12 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">

</xml_diff>